<commit_message>
fix the few problems in compliant info
</commit_message>
<xml_diff>
--- a/Adaptor_combined_result.xlsx
+++ b/Adaptor_combined_result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,708 +436,1677 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Adaptor Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Connector 1 Type</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Connector 1 Impedance</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Connector 1 Polarity</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Connector 2 Type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Connector 2 Impedance</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Connector 2 Polarity</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Connector Mount Method</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Adapter Body Style</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Insertion Loss (dB)</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>VSWR /Return Loss</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Center Contact</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Outer Contact</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Body</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Dielectric</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Temperature Range</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>2011/65/EU(RoHS)</t>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Compliant</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1.0mm Male</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>1.85/GPPO-JK</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>50 Ohms</t>
+          <t>1.85mm Male</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Standard</t>
+          <t>50 Ohms</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.8mm Male</t>
+          <t>Standard</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>50 Ohms</t>
+          <t>GPPO(MINI-SMP) Female</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Standard</t>
+          <t>50 Ohms</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>DC to 110 GHz</t>
+          <t>Straight</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>≤0.5</t>
+          <t xml:space="preserve">
+DC to 67 GHz</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>≤ 0.08 xSqt.(f_GHz)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t xml:space="preserve">
+1.3</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>CuBe Gold Plated</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Stainless Steel</t>
-        </is>
-      </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Straight</t>
+          <t>CuBe Gold Plated</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>PEI</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>-45°C to +125°C</t>
-        </is>
-      </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Compliant</t>
+          <t xml:space="preserve">  
+-40°C to +85°C</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2002/95/EC(RoHS) </t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>1.0/0.8-JJS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1.0mm Male</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>0.8mm Male</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>DC to 110 GHz</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>≤0.5</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>-45°C to +125°C</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>1.85/G3PO-KJ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.85mm Female</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>G3PO(SMPS) Male</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>DC to 67 GHz</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>≤0.08 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>1.35 to 67 GHz</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>-45°C to +125°C</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>0.8-JKS</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0.8mm Male</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>0.8mm Female</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t xml:space="preserve">
 DC to 145 GHz</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>≤ 0.05 xSqt.(f_GHz)</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t xml:space="preserve">
 1.60</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>CuBe Gold Plated</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
         <is>
           <t>PEI</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t xml:space="preserve">  
 -40°C to +85°C</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2011/65/EU(RoHS) </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>1.85/1.0-KJS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.0mm Male</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1.85mm Female</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>DC to 67 GHz</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>≤0.05 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>1.30 to 67 GHz</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>CuBe  Gold Plated</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>-55°C to +165°C</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>2002/95/EC(RoHS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>1.85/G3PO-KK</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1.85mm Female</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>G3PO(SMPS) Female</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Compliant</t>
+DC to 65 GHz</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>≤ 0.05 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+1.35 to 65 GHz</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>CuBe  Gold Plated</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  
+-40°C to +85°C</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2002/95/EC(RoHS) </t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>1.85/G3PO-JJ</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1.85mm Male</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>G3PO(SMPS) Male</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>DC to 67 GHz</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>≤0.08 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>1.35 to 67 GHz</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated &amp; Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>-45°C to +125°C</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>0.8-JJS</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>0.8mm Male</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>0.8mm Male</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t xml:space="preserve">
 DC to 145 GHz</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>≤ 0.05 xSqt.(f_GHz)</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t xml:space="preserve">
 1.60</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>CuBe Gold Plated</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
         <is>
           <t>PEI</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t xml:space="preserve">  
 -40°C to +85°C</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="R9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2011/65/EU(RoHS) </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>1.0/0.8-JKS</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1.0mm Male</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.8mm Female</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>DC to 110 GHz</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>≤0.5</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>-45°C to +125°C</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>1.85/GPPO-KJ</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1.85mm Female</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>GPPO(MINI-SMP) Male</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Compliant</t>
+DC to 67 GHz</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>≤ 0.08 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+1.3</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  
+-40°C to +85°C</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2011/65/EU(RoHS) </t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1.0mm Male</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>1.85/1.0-KKS</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1.0mm Female</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1.85mm Female</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+DC to 67 GHz</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>≤ 0.05 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+1.30 to 67 GHz</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>CuBe  Gold Plated</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  
+-55°C to +165°C</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2002/95/EC(RoHS) </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>1.85/G3PO-JK</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1.85mm Male</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>G3PO(SMPS) Female</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>DC to 67 GHz</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>≤0.08 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>1.35 to 67 GHz</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated &amp; Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>-45°C to +125°C</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>0.8-KKS</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>0.8mm Female</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0.8mm Female</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>DC to 110 GHz</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>≤0.5</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>1.5</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>CuBe Gold Plated</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Stainless Steel</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>PEI</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>-45°C to +125°C</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Compliant</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>0.8mm Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0.8mm Female</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
         <is>
           <t xml:space="preserve">
 DC to 145 GHz</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>≤ 0.05 xSqt.(f_GHz)</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t xml:space="preserve">
 1.60</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>CuBe Gold Plated</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
         <is>
           <t>PEI</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t xml:space="preserve">  
 -40°C to +85°C</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Compliant</t>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2011/65/EU(RoHS) </t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>1.0/0.8-KJS</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>1.0mm Female</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>0.8mm Male</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>DC to 110 GHz</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>≤0.5</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>1.5</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>CuBe Gold Plated</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
         <is>
           <t>PEI</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>-45°C to +125°C</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>Compliant</t>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>1.85/1.0-JJS</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1.85mm Male</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1.0MM Male</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>DC to 67 GHz</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>≤0.08 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>1.30 to 67 GHz</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>-45°C to +125°C</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>1.0/0.8-KKS</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>1.0mm Female</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>0.8mm Female</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>50 Ohms</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
         <is>
           <t>DC to 110 GHz</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>≤0.5</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>1.5</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>CuBe Gold Plated</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>Straight</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
         <is>
           <t>PEI</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>-45°C to +125°C</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Compliant</t>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>1.85/1.0-JKS</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1.85mm Male</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1.0MM Male</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>50 Ohms</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>DC to 67 GHz</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>≤0.08 xSqt.(f_GHz)</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>1.30 to 67 GHz</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>CuBe Gold Plated &amp; Stainless Steel</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Straight</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>PEI</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>-45°C to +125°C</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>2011/65/EU(RoHS)</t>
         </is>
       </c>
     </row>

</xml_diff>